<commit_message>
edits (mostly to the excel)
</commit_message>
<xml_diff>
--- a/sortexcel.xlsx
+++ b/sortexcel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" state="visible" r:id="rId3"/>
@@ -4153,8 +4153,8 @@
   </sheetPr>
   <dimension ref="A1:W43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K22" activeCellId="0" sqref="K22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J18" activeCellId="0" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5290,9 +5290,9 @@
   <dimension ref="A1:P499"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G160" activeCellId="0" sqref="G160"/>
+      <selection pane="bottomLeft" activeCell="L92" activeCellId="0" sqref="L92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12336,22 +12336,22 @@
       <c r="B196" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="C196" s="0" t="n">
+      <c r="C196" s="1" t="n">
         <v>90</v>
       </c>
-      <c r="D196" s="0" t="n">
+      <c r="D196" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="E196" s="0" t="n">
+      <c r="E196" s="1" t="n">
         <v>85</v>
       </c>
-      <c r="F196" s="0" t="n">
+      <c r="F196" s="1" t="n">
         <v>105</v>
       </c>
-      <c r="G196" s="0" t="n">
+      <c r="G196" s="1" t="n">
         <v>120</v>
       </c>
-      <c r="H196" s="0" t="n">
+      <c r="H196" s="1" t="n">
         <v>120</v>
       </c>
       <c r="I196" s="9" t="s">
@@ -12372,22 +12372,22 @@
       <c r="B197" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="C197" s="0" t="n">
+      <c r="C197" s="1" t="n">
         <v>70</v>
       </c>
-      <c r="D197" s="0" t="n">
+      <c r="D197" s="1" t="n">
         <v>70</v>
       </c>
-      <c r="E197" s="0" t="n">
+      <c r="E197" s="1" t="n">
         <v>120</v>
       </c>
-      <c r="F197" s="0" t="n">
+      <c r="F197" s="1" t="n">
         <v>120</v>
       </c>
-      <c r="G197" s="0" t="n">
+      <c r="G197" s="1" t="n">
         <v>125</v>
       </c>
-      <c r="H197" s="0" t="n">
+      <c r="H197" s="1" t="n">
         <v>75</v>
       </c>
       <c r="I197" s="9" t="s">
@@ -12408,22 +12408,22 @@
       <c r="B198" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="C198" s="0" t="n">
+      <c r="C198" s="1" t="n">
         <v>120</v>
       </c>
-      <c r="D198" s="0" t="n">
+      <c r="D198" s="1" t="n">
         <v>70</v>
       </c>
-      <c r="E198" s="0" t="n">
+      <c r="E198" s="1" t="n">
         <v>75</v>
       </c>
-      <c r="F198" s="0" t="n">
+      <c r="F198" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="G198" s="0" t="n">
+      <c r="G198" s="1" t="n">
         <v>120</v>
       </c>
-      <c r="H198" s="0" t="n">
+      <c r="H198" s="1" t="n">
         <v>95</v>
       </c>
       <c r="I198" s="9" t="s">
@@ -12444,22 +12444,22 @@
       <c r="B199" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="C199" s="0" t="n">
+      <c r="C199" s="1" t="n">
         <v>110</v>
       </c>
-      <c r="D199" s="0" t="n">
+      <c r="D199" s="1" t="n">
         <v>85</v>
       </c>
-      <c r="E199" s="0" t="n">
+      <c r="E199" s="1" t="n">
         <v>125</v>
       </c>
-      <c r="F199" s="0" t="n">
+      <c r="F199" s="1" t="n">
         <v>55</v>
       </c>
-      <c r="G199" s="0" t="n">
+      <c r="G199" s="1" t="n">
         <v>90</v>
       </c>
-      <c r="H199" s="0" t="n">
+      <c r="H199" s="1" t="n">
         <v>115</v>
       </c>
       <c r="I199" s="9" t="s">
@@ -12480,22 +12480,22 @@
       <c r="B200" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="C200" s="0" t="n">
+      <c r="C200" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="D200" s="0" t="n">
+      <c r="D200" s="1" t="n">
         <v>130</v>
       </c>
-      <c r="E200" s="0" t="n">
+      <c r="E200" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="F200" s="0" t="n">
+      <c r="F200" s="1" t="n">
         <v>150</v>
       </c>
-      <c r="G200" s="0" t="n">
+      <c r="G200" s="1" t="n">
         <v>140</v>
       </c>
-      <c r="H200" s="0" t="n">
+      <c r="H200" s="1" t="n">
         <v>80</v>
       </c>
       <c r="I200" s="9" t="s">
@@ -12516,22 +12516,22 @@
       <c r="B201" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="C201" s="0" t="n">
+      <c r="C201" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="D201" s="0" t="n">
+      <c r="D201" s="1" t="n">
         <v>150</v>
       </c>
-      <c r="E201" s="0" t="n">
+      <c r="E201" s="1" t="n">
         <v>140</v>
       </c>
-      <c r="F201" s="0" t="n">
+      <c r="F201" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="G201" s="0" t="n">
+      <c r="G201" s="1" t="n">
         <v>130</v>
       </c>
-      <c r="H201" s="0" t="n">
+      <c r="H201" s="1" t="n">
         <v>80</v>
       </c>
       <c r="I201" s="9" t="s">
@@ -12552,22 +12552,22 @@
       <c r="B202" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="C202" s="0" t="n">
+      <c r="C202" s="1" t="n">
         <v>110</v>
       </c>
-      <c r="D202" s="0" t="n">
+      <c r="D202" s="1" t="n">
         <v>85</v>
       </c>
-      <c r="E202" s="0" t="n">
+      <c r="E202" s="1" t="n">
         <v>140</v>
       </c>
-      <c r="F202" s="0" t="n">
+      <c r="F202" s="1" t="n">
         <v>85</v>
       </c>
-      <c r="G202" s="0" t="n">
+      <c r="G202" s="1" t="n">
         <v>110</v>
       </c>
-      <c r="H202" s="0" t="n">
+      <c r="H202" s="1" t="n">
         <v>150</v>
       </c>
       <c r="I202" s="9" t="s">
@@ -12588,22 +12588,22 @@
       <c r="B203" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="C203" s="0" t="n">
+      <c r="C203" s="1" t="n">
         <v>124</v>
       </c>
-      <c r="D203" s="0" t="n">
+      <c r="D203" s="1" t="n">
         <v>153</v>
       </c>
-      <c r="E203" s="0" t="n">
+      <c r="E203" s="1" t="n">
         <v>112</v>
       </c>
-      <c r="F203" s="0" t="n">
+      <c r="F203" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="G203" s="0" t="n">
+      <c r="G203" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="H203" s="0" t="n">
+      <c r="H203" s="1" t="n">
         <v>94</v>
       </c>
       <c r="I203" s="9" t="s">
@@ -12624,22 +12624,22 @@
       <c r="B204" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="C204" s="0" t="n">
+      <c r="C204" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="D204" s="0" t="n">
+      <c r="D204" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="E204" s="0" t="n">
+      <c r="E204" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="F204" s="0" t="n">
+      <c r="F204" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="G204" s="0" t="n">
+      <c r="G204" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="H204" s="0" t="n">
+      <c r="H204" s="1" t="n">
         <v>100</v>
       </c>
       <c r="I204" s="9" t="s">
@@ -12660,22 +12660,22 @@
       <c r="B205" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="C205" s="0" t="n">
+      <c r="C205" s="1" t="n">
         <v>48</v>
       </c>
-      <c r="D205" s="0" t="n">
+      <c r="D205" s="1" t="n">
         <v>48</v>
       </c>
-      <c r="E205" s="0" t="n">
+      <c r="E205" s="1" t="n">
         <v>48</v>
       </c>
-      <c r="F205" s="0" t="n">
+      <c r="F205" s="1" t="n">
         <v>48</v>
       </c>
-      <c r="G205" s="0" t="n">
+      <c r="G205" s="1" t="n">
         <v>48</v>
       </c>
-      <c r="H205" s="0" t="n">
+      <c r="H205" s="1" t="n">
         <v>48</v>
       </c>
       <c r="I205" s="9" t="s">
@@ -14469,9 +14469,9 @@
   <dimension ref="A1:P499"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A188" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="K205" activeCellId="0" sqref="K205"/>
+      <selection pane="bottomLeft" activeCell="J212" activeCellId="0" sqref="J212"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -23388,22 +23388,22 @@
       <c r="B248" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="C248" s="0" t="n">
+      <c r="C248" s="1" t="n">
         <v>94</v>
       </c>
-      <c r="D248" s="0" t="n">
+      <c r="D248" s="1" t="n">
         <v>43</v>
       </c>
-      <c r="E248" s="0" t="n">
+      <c r="E248" s="1" t="n">
         <v>140</v>
       </c>
-      <c r="F248" s="0" t="n">
+      <c r="F248" s="1" t="n">
         <v>29</v>
       </c>
-      <c r="G248" s="0" t="n">
+      <c r="G248" s="1" t="n">
         <v>62</v>
       </c>
-      <c r="H248" s="0" t="n">
+      <c r="H248" s="1" t="n">
         <v>130</v>
       </c>
       <c r="I248" s="9" t="s">
@@ -23424,22 +23424,22 @@
       <c r="B249" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="C249" s="0" t="n">
+      <c r="C249" s="1" t="n">
         <v>69</v>
       </c>
-      <c r="D249" s="0" t="n">
+      <c r="D249" s="1" t="n">
         <v>69</v>
       </c>
-      <c r="E249" s="0" t="n">
+      <c r="E249" s="1" t="n">
         <v>117</v>
       </c>
-      <c r="F249" s="0" t="n">
+      <c r="F249" s="1" t="n">
         <v>49</v>
       </c>
-      <c r="G249" s="0" t="n">
+      <c r="G249" s="1" t="n">
         <v>69</v>
       </c>
-      <c r="H249" s="0" t="n">
+      <c r="H249" s="1" t="n">
         <v>117</v>
       </c>
       <c r="I249" s="9" t="s">
@@ -23463,22 +23463,22 @@
       <c r="B250" s="1" t="s">
         <v>302</v>
       </c>
-      <c r="C250" s="0" t="n">
+      <c r="C250" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="D250" s="0" t="n">
+      <c r="D250" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="E250" s="0" t="n">
+      <c r="E250" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="F250" s="0" t="n">
+      <c r="F250" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="G250" s="0" t="n">
+      <c r="G250" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="H250" s="0" t="n">
+      <c r="H250" s="1" t="n">
         <v>80</v>
       </c>
       <c r="I250" s="9" t="s">
@@ -23496,22 +23496,22 @@
       <c r="B251" s="1" t="s">
         <v>303</v>
       </c>
-      <c r="C251" s="0" t="n">
+      <c r="C251" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="D251" s="0" t="n">
+      <c r="D251" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="E251" s="0" t="n">
+      <c r="E251" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="F251" s="0" t="n">
+      <c r="F251" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="G251" s="0" t="n">
+      <c r="G251" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="H251" s="0" t="n">
+      <c r="H251" s="1" t="n">
         <v>80</v>
       </c>
       <c r="I251" s="9" t="s">
@@ -23529,22 +23529,22 @@
       <c r="B252" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="C252" s="0" t="n">
+      <c r="C252" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="D252" s="0" t="n">
+      <c r="D252" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="E252" s="0" t="n">
+      <c r="E252" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="F252" s="0" t="n">
+      <c r="F252" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="G252" s="0" t="n">
+      <c r="G252" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="H252" s="0" t="n">
+      <c r="H252" s="1" t="n">
         <v>80</v>
       </c>
       <c r="I252" s="9" t="s">
@@ -23562,22 +23562,22 @@
       <c r="B253" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="C253" s="0" t="n">
+      <c r="C253" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="D253" s="0" t="n">
+      <c r="D253" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="E253" s="0" t="n">
+      <c r="E253" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="F253" s="0" t="n">
+      <c r="F253" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="G253" s="0" t="n">
+      <c r="G253" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="H253" s="0" t="n">
+      <c r="H253" s="1" t="n">
         <v>80</v>
       </c>
       <c r="I253" s="9" t="s">
@@ -23595,22 +23595,22 @@
       <c r="B254" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="C254" s="0" t="n">
+      <c r="C254" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="D254" s="0" t="n">
+      <c r="D254" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="E254" s="0" t="n">
+      <c r="E254" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="F254" s="0" t="n">
+      <c r="F254" s="1" t="n">
         <v>50</v>
       </c>
-      <c r="G254" s="0" t="n">
+      <c r="G254" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="H254" s="0" t="n">
+      <c r="H254" s="1" t="n">
         <v>25</v>
       </c>
       <c r="I254" s="9" t="s">
@@ -23631,22 +23631,22 @@
       <c r="B255" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="C255" s="0" t="n">
+      <c r="C255" s="1" t="n">
         <v>95</v>
       </c>
-      <c r="D255" s="0" t="n">
+      <c r="D255" s="1" t="n">
         <v>155</v>
       </c>
-      <c r="E255" s="0" t="n">
+      <c r="E255" s="1" t="n">
         <v>109</v>
       </c>
-      <c r="F255" s="0" t="n">
+      <c r="F255" s="1" t="n">
         <v>81</v>
       </c>
-      <c r="G255" s="0" t="n">
+      <c r="G255" s="1" t="n">
         <v>70</v>
       </c>
-      <c r="H255" s="0" t="n">
+      <c r="H255" s="1" t="n">
         <v>130</v>
       </c>
       <c r="I255" s="9" t="s">
@@ -23670,22 +23670,22 @@
       <c r="B256" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="C256" s="0" t="n">
+      <c r="C256" s="1" t="n">
         <v>85</v>
       </c>
-      <c r="D256" s="0" t="n">
+      <c r="D256" s="1" t="n">
         <v>89</v>
       </c>
-      <c r="E256" s="0" t="n">
+      <c r="E256" s="1" t="n">
         <v>125</v>
       </c>
-      <c r="F256" s="0" t="n">
+      <c r="F256" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="G256" s="0" t="n">
+      <c r="G256" s="1" t="n">
         <v>91</v>
       </c>
-      <c r="H256" s="0" t="n">
+      <c r="H256" s="1" t="n">
         <v>90</v>
       </c>
       <c r="I256" s="9" t="s">
@@ -23709,22 +23709,22 @@
       <c r="B257" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="C257" s="0" t="n">
+      <c r="C257" s="1" t="n">
         <v>74</v>
       </c>
-      <c r="D257" s="0" t="n">
+      <c r="D257" s="1" t="n">
         <v>65</v>
       </c>
-      <c r="E257" s="0" t="n">
+      <c r="E257" s="1" t="n">
         <v>67</v>
       </c>
-      <c r="F257" s="0" t="n">
+      <c r="F257" s="1" t="n">
         <v>92</v>
       </c>
-      <c r="G257" s="0" t="n">
+      <c r="G257" s="1" t="n">
         <v>125</v>
       </c>
-      <c r="H257" s="0" t="n">
+      <c r="H257" s="1" t="n">
         <v>128</v>
       </c>
       <c r="I257" s="9" t="s">
@@ -25205,10 +25205,10 @@
   </sheetPr>
   <dimension ref="A1:L310"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="B229" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="B2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F247" activeCellId="0" sqref="F247"/>
+      <selection pane="bottomLeft" activeCell="I14" activeCellId="0" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -76226,14 +76226,6 @@
         <v>455</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0"/>
-      <c r="L6" s="0"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="0"/>
-      <c r="L7" s="0"/>
-    </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <v>536</v>

</xml_diff>

<commit_message>
failsafe update and excel (again)
</commit_message>
<xml_diff>
--- a/sortexcel.xlsx
+++ b/sortexcel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" state="visible" r:id="rId3"/>
@@ -4153,8 +4153,8 @@
   </sheetPr>
   <dimension ref="A1:W43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J18" activeCellId="0" sqref="J18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J24" activeCellId="0" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5289,10 +5289,10 @@
   </sheetPr>
   <dimension ref="A1:P499"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A158" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="L92" activeCellId="0" sqref="L92"/>
+      <selection pane="bottomLeft" activeCell="L172" activeCellId="0" sqref="L172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14469,9 +14469,9 @@
   <dimension ref="A1:P499"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A188" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="J212" activeCellId="0" sqref="J212"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -25205,10 +25205,10 @@
   </sheetPr>
   <dimension ref="A1:L310"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="B2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I14" activeCellId="0" sqref="I14"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -38616,8 +38616,8 @@
   </sheetPr>
   <dimension ref="A1:P1082"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A896" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A907" activeCellId="0" sqref="A907"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>